<commit_message>
old project without accounts
</commit_message>
<xml_diff>
--- a/acs_coffee_management/2024-09-13_employees.xlsx
+++ b/acs_coffee_management/2024-09-13_employees.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="231">
   <si>
     <t>_state</t>
   </si>
@@ -40,166 +40,175 @@
     <t>updated_at</t>
   </si>
   <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9B80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9C40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9D00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9DC0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9E80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9F40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B9FD0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3100&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B31C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3280&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3340&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3400&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B34C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3580&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3640&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3700&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B37C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3880&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3940&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3A00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3AC0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3B80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3C40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3D00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3DC0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3E80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3F40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17B3FD0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790100&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17901C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790280&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790340&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790400&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17904C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790580&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790640&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790700&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED17907C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790880&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790940&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790A00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790AC0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790B80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790C40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790D00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790DC0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790E80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790F40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED1790FD0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED19A1100&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED19A11C0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED19A1280&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED19A1340&gt;</t>
-  </si>
-  <si>
-    <t>&lt;django.db.models.base.ModelState object at 0x0000023ED19A1400&gt;</t>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C00A0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C0490&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C0760&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C0700&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C02E0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C0310&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C0C40&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05C0880&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3EB0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3EE0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F35B0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F33A0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F36D0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3760&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3940&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3970&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3D90&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3A00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3130&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3FD0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3DF0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3640&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04F3520&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473C10&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473BE0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473CA0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473D60&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473E20&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473EB0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473FA0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473F40&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D0473FD0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD850&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD190&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD790&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD880&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDB50&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD250&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD220&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD5B0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDA90&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD910&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD4F0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD040&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDCA0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD4C0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD730&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDBB0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD7F0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDE80&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD160&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDDF0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD610&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD7C0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BD970&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D04BDAF0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;django.db.models.base.ModelState object at 0x00000298D05BBF40&gt;</t>
   </si>
   <si>
     <t>Acosta, Andres</t>
@@ -286,6 +295,9 @@
     <t>Lenz, Lukas</t>
   </si>
   <si>
+    <t>Max</t>
+  </si>
+  <si>
     <t>Monti, Antonello</t>
   </si>
   <si>
@@ -340,6 +352,9 @@
     <t>Stoyanova, Ivelina</t>
   </si>
   <si>
+    <t>Test, test</t>
+  </si>
+  <si>
     <t>Tun, Su Mon</t>
   </si>
   <si>
@@ -364,6 +379,9 @@
     <t>Yavuzer, Arty</t>
   </si>
   <si>
+    <t>saddsa</t>
+  </si>
+  <si>
     <t>qr-1</t>
   </si>
   <si>
@@ -448,6 +466,9 @@
     <t>qr-21</t>
   </si>
   <si>
+    <t>max</t>
+  </si>
+  <si>
     <t>qr-22</t>
   </si>
   <si>
@@ -502,6 +523,9 @@
     <t>qr-34</t>
   </si>
   <si>
+    <t>test-test</t>
+  </si>
+  <si>
     <t>qr-50</t>
   </si>
   <si>
@@ -526,115 +550,163 @@
     <t>qr-37</t>
   </si>
   <si>
+    <t>sdasda</t>
+  </si>
+  <si>
     <t>nan</t>
   </si>
   <si>
+    <t>max.mustermann@web.de</t>
+  </si>
+  <si>
+    <t>test@wreb.de</t>
+  </si>
+  <si>
+    <t>sdasda@web.de</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>1.40</t>
+  </si>
+  <si>
+    <t>33.30</t>
+  </si>
+  <si>
+    <t>50.80</t>
+  </si>
+  <si>
+    <t>-16.14</t>
+  </si>
+  <si>
+    <t>22.40</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>19.20</t>
+  </si>
+  <si>
+    <t>12.60</t>
+  </si>
+  <si>
     <t>0.60</t>
   </si>
   <si>
-    <t>0.90</t>
-  </si>
-  <si>
-    <t>10.50</t>
-  </si>
-  <si>
-    <t>19.20</t>
-  </si>
-  <si>
-    <t>-25.74</t>
-  </si>
-  <si>
-    <t>0.00</t>
+    <t>10.90</t>
+  </si>
+  <si>
+    <t>7.40</t>
+  </si>
+  <si>
+    <t>-0.50</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>4.30</t>
+  </si>
+  <si>
+    <t>22.50</t>
+  </si>
+  <si>
+    <t>27.20</t>
+  </si>
+  <si>
+    <t>26.70</t>
+  </si>
+  <si>
+    <t>18.30</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>15.05</t>
+  </si>
+  <si>
+    <t>47.90</t>
+  </si>
+  <si>
+    <t>58.65</t>
+  </si>
+  <si>
+    <t>77.10</t>
+  </si>
+  <si>
+    <t>8.20</t>
+  </si>
+  <si>
+    <t>7.00</t>
+  </si>
+  <si>
+    <t>5.30</t>
+  </si>
+  <si>
+    <t>8.90</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>14.90</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>3.45</t>
+  </si>
+  <si>
+    <t>35.60</t>
+  </si>
+  <si>
+    <t>-3.40</t>
   </si>
   <si>
     <t>0.40</t>
   </si>
   <si>
-    <t>12.60</t>
-  </si>
-  <si>
-    <t>7.40</t>
-  </si>
-  <si>
-    <t>-10.10</t>
-  </si>
-  <si>
-    <t>0.30</t>
-  </si>
-  <si>
-    <t>0.70</t>
-  </si>
-  <si>
-    <t>2.90</t>
-  </si>
-  <si>
-    <t>2.70</t>
-  </si>
-  <si>
-    <t>17.50</t>
-  </si>
-  <si>
-    <t>9.45</t>
-  </si>
-  <si>
-    <t>25.50</t>
-  </si>
-  <si>
-    <t>46.65</t>
-  </si>
-  <si>
-    <t>7.80</t>
-  </si>
-  <si>
-    <t>1.20</t>
-  </si>
-  <si>
-    <t>1.40</t>
-  </si>
-  <si>
-    <t>3.40</t>
-  </si>
-  <si>
-    <t>8.50</t>
-  </si>
-  <si>
-    <t>6.00</t>
-  </si>
-  <si>
-    <t>-5.50</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>2.25</t>
-  </si>
-  <si>
-    <t>-4.20</t>
-  </si>
-  <si>
-    <t>3.00</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>1.35</t>
-  </si>
-  <si>
-    <t>-2.25</t>
+    <t>5.15</t>
+  </si>
+  <si>
+    <t>3.75</t>
+  </si>
+  <si>
+    <t>3.35</t>
   </si>
   <si>
     <t>2.35</t>
   </si>
   <si>
-    <t>1.90</t>
-  </si>
-  <si>
-    <t>-22.00</t>
-  </si>
-  <si>
-    <t>3.25</t>
+    <t>6.70</t>
+  </si>
+  <si>
+    <t>2.40</t>
+  </si>
+  <si>
+    <t>-20.40</t>
+  </si>
+  <si>
+    <t>3.85</t>
+  </si>
+  <si>
+    <t>6.45</t>
+  </si>
+  <si>
+    <t>0.80</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1068,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1039,22 +1111,22 @@
         <v>348</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2">
-        <v>45548.40434677215</v>
+        <v>45548.82629091716</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1068,22 +1140,22 @@
         <v>349</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>45548.40434701156</v>
+        <v>45548.8262911518</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1097,22 +1169,22 @@
         <v>350</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G4" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>45548.40434711573</v>
+        <v>45548.82629136405</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1126,22 +1198,22 @@
         <v>351</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="F5" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G5" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="H5">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>45548.40434721213</v>
+        <v>45548.82629155905</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1155,22 +1227,22 @@
         <v>352</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="H6">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>45548.40434730465</v>
+        <v>45548.82629177103</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1184,22 +1256,22 @@
         <v>353</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G7" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="H7">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>45548.404347396</v>
+        <v>45548.82629197925</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1213,22 +1285,22 @@
         <v>354</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G8" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H8">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>45548.4043474767</v>
+        <v>45548.82629220819</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1242,22 +1314,22 @@
         <v>355</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G9" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <v>45548.40434755619</v>
+        <v>45548.82629242536</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1271,22 +1343,22 @@
         <v>356</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G10" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="H10">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>45548.40434755619</v>
+        <v>45548.82629264552</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1300,22 +1372,22 @@
         <v>357</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G11" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <v>45548.40434777043</v>
+        <v>45548.82629287663</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1329,22 +1401,22 @@
         <v>358</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G12" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>45548.40434786301</v>
+        <v>45548.82629309039</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1358,22 +1430,22 @@
         <v>359</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F13" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G13" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="H13">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>45548.40434795706</v>
+        <v>45548.82629329022</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1387,22 +1459,22 @@
         <v>360</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G14" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>45548.4043480496</v>
+        <v>45548.82629350551</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1416,22 +1488,22 @@
         <v>361</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F15" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" s="2">
-        <v>45548.40434810706</v>
+        <v>45548.82629371303</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1445,22 +1517,22 @@
         <v>362</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F16" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G16" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="H16">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>45548.40434810706</v>
+        <v>45548.82629388534</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1474,22 +1546,22 @@
         <v>363</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F17" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G17" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="H17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I17" s="2">
-        <v>45548.40434832014</v>
+        <v>45548.82629411463</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1503,22 +1575,22 @@
         <v>364</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G18" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>45548.40434832014</v>
+        <v>45548.82629434356</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1532,22 +1604,22 @@
         <v>365</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F19" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G19" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="H19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>45548.40434853605</v>
+        <v>45548.82629453261</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1561,22 +1633,22 @@
         <v>366</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G20" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20" s="2">
-        <v>45548.40434861693</v>
+        <v>45548.82629472734</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1590,22 +1662,22 @@
         <v>367</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E21" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G21" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="H21">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="I21" s="2">
-        <v>45548.40434872653</v>
+        <v>45548.82629492225</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1619,22 +1691,22 @@
         <v>368</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F22" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G22" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="H22">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
-        <v>45548.40434881942</v>
+        <v>45548.82629513008</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1648,22 +1720,22 @@
         <v>369</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F23" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G23" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="H23">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>45548.40434888139</v>
+        <v>45548.8262953611</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1677,22 +1749,22 @@
         <v>370</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F24" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G24" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2">
-        <v>45548.40434888139</v>
+        <v>45548.82629558085</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1706,22 +1778,22 @@
         <v>371</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2">
-        <v>45548.4043490957</v>
+        <v>45548.82629578577</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1735,22 +1807,22 @@
         <v>372</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F26" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G26" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I26" s="2">
-        <v>45548.4043490957</v>
+        <v>45548.82629599769</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1764,22 +1836,22 @@
         <v>373</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G27" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="H27">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I27" s="2">
-        <v>45548.40434932624</v>
+        <v>45548.82629620202</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1793,22 +1865,22 @@
         <v>374</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G28" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="H28">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>45548.40434941889</v>
+        <v>45548.82629639627</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1822,22 +1894,22 @@
         <v>375</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F29" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G29" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="H29">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2">
-        <v>45548.40434948293</v>
+        <v>45548.82629657983</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1848,25 +1920,25 @@
         <v>36</v>
       </c>
       <c r="C30">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F30" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G30" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="2">
-        <v>45548.40434948293</v>
+        <v>45548.82629679477</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1877,25 +1949,25 @@
         <v>37</v>
       </c>
       <c r="C31">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F31" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G31" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <v>45548.40434971116</v>
+        <v>45548.82629697426</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1906,25 +1978,25 @@
         <v>38</v>
       </c>
       <c r="C32">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F32" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G32" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32" s="2">
-        <v>45548.40434980404</v>
+        <v>45548.82629718376</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1935,25 +2007,25 @@
         <v>39</v>
       </c>
       <c r="C33">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F33" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H33">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I33" s="2">
-        <v>45548.40434989635</v>
+        <v>45548.82629737216</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1964,25 +2036,25 @@
         <v>40</v>
       </c>
       <c r="C34">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F34" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G34" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="H34">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>45548.404349989</v>
+        <v>45548.8262975795</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1993,25 +2065,25 @@
         <v>41</v>
       </c>
       <c r="C35">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F35" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G35" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="2">
-        <v>45548.40435003638</v>
+        <v>45548.8262977719</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2022,25 +2094,25 @@
         <v>42</v>
       </c>
       <c r="C36">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F36" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G36" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36" s="2">
-        <v>45548.40435003638</v>
+        <v>45548.82629795566</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2051,25 +2123,25 @@
         <v>43</v>
       </c>
       <c r="C37">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="F37" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G37" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="H37">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>45548.40435024473</v>
+        <v>45548.826298137</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2080,25 +2152,25 @@
         <v>44</v>
       </c>
       <c r="C38">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E38" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F38" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G38" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I38" s="2">
-        <v>45548.40435024473</v>
+        <v>45548.82629833496</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2109,25 +2181,25 @@
         <v>45</v>
       </c>
       <c r="C39">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F39" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G39" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I39" s="2">
-        <v>45548.40435048167</v>
+        <v>45548.82629851752</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2138,25 +2210,25 @@
         <v>46</v>
       </c>
       <c r="C40">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D40" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F40" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G40" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I40" s="2">
-        <v>45548.40435056265</v>
+        <v>45548.82629871297</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2167,25 +2239,25 @@
         <v>47</v>
       </c>
       <c r="C41">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E41" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F41" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G41" t="s">
-        <v>176</v>
+        <v>217</v>
       </c>
       <c r="H41">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="I41" s="2">
-        <v>45548.40435066712</v>
+        <v>45548.82629888795</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2196,25 +2268,25 @@
         <v>48</v>
       </c>
       <c r="C42">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E42" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F42" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G42" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42" s="2">
-        <v>45548.40435075971</v>
+        <v>45548.82629907388</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2225,25 +2297,25 @@
         <v>49</v>
       </c>
       <c r="C43">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D43" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E43" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F43" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G43" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>45548.40435080825</v>
+        <v>45548.8262992972</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2254,25 +2326,25 @@
         <v>50</v>
       </c>
       <c r="C44">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D44" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E44" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F44" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G44" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="H44">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I44" s="2">
-        <v>45548.40435080825</v>
+        <v>45548.82629947811</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2283,25 +2355,25 @@
         <v>51</v>
       </c>
       <c r="C45">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E45" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F45" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G45" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="2">
-        <v>45548.4043510168</v>
+        <v>45548.82629966312</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2312,25 +2384,25 @@
         <v>52</v>
       </c>
       <c r="C46">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="F46" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G46" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H46">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I46" s="2">
-        <v>45548.40435110948</v>
+        <v>45548.82629987392</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2341,25 +2413,25 @@
         <v>53</v>
       </c>
       <c r="C47">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F47" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G47" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="H47">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I47" s="2">
-        <v>45548.40435124149</v>
+        <v>45548.82630005368</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2370,25 +2442,25 @@
         <v>54</v>
       </c>
       <c r="C48">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G48" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="H48">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I48" s="2">
-        <v>45548.4043513221</v>
+        <v>45548.82630026139</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2399,25 +2471,25 @@
         <v>55</v>
       </c>
       <c r="C49">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="D49" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="F49" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="G49" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49" s="2">
-        <v>45548.40435144154</v>
+        <v>45548.82630046055</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2428,25 +2500,25 @@
         <v>56</v>
       </c>
       <c r="C50">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E50" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F50" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G50" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="H50">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I50" s="2">
-        <v>45548.40435152256</v>
+        <v>45548.82630063411</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2457,25 +2529,25 @@
         <v>57</v>
       </c>
       <c r="C51">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E51" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F51" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G51" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
       <c r="H51">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I51" s="2">
-        <v>45548.40435158081</v>
+        <v>45548.82630085801</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2486,25 +2558,25 @@
         <v>58</v>
       </c>
       <c r="C52">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D52" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E52" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F52" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G52" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I52" s="2">
-        <v>45548.40435158081</v>
+        <v>45548.82630104657</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2515,25 +2587,25 @@
         <v>59</v>
       </c>
       <c r="C53">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D53" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E53" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F53" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G53" t="s">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I53" s="2">
-        <v>45548.4043517959</v>
+        <v>45548.82630126715</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2544,25 +2616,25 @@
         <v>60</v>
       </c>
       <c r="C54">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D54" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E54" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F54" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="G54" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="H54">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I54" s="2">
-        <v>45548.40435191177</v>
+        <v>45548.8263014622</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2573,25 +2645,112 @@
         <v>61</v>
       </c>
       <c r="C55">
+        <v>399</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s">
+        <v>175</v>
+      </c>
+      <c r="F55" t="s">
+        <v>179</v>
+      </c>
+      <c r="G55" t="s">
+        <v>228</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2">
+        <v>45548.82630162893</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56">
+        <v>400</v>
+      </c>
+      <c r="D56" t="s">
+        <v>119</v>
+      </c>
+      <c r="E56" t="s">
+        <v>176</v>
+      </c>
+      <c r="F56" t="s">
+        <v>179</v>
+      </c>
+      <c r="G56" t="s">
+        <v>229</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2">
+        <v>45548.8263018387</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57">
         <v>401</v>
       </c>
-      <c r="D55" t="s">
-        <v>115</v>
-      </c>
-      <c r="E55" t="s">
-        <v>169</v>
-      </c>
-      <c r="F55" t="s">
-        <v>170</v>
-      </c>
-      <c r="G55" t="s">
-        <v>176</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2">
-        <v>45548.40435201617</v>
+      <c r="D57" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" t="s">
+        <v>177</v>
+      </c>
+      <c r="F57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G57" t="s">
+        <v>190</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2">
+        <v>45548.82630204195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <v>402</v>
+      </c>
+      <c r="D58" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" t="s">
+        <v>178</v>
+      </c>
+      <c r="F58" t="s">
+        <v>182</v>
+      </c>
+      <c r="G58" t="s">
+        <v>230</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <v>45548.82630221278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>